<commit_message>
Add enigma summary stats file
</commit_message>
<xml_diff>
--- a/data/ENIGMA/ENIGMA_structural_organised.xlsx
+++ b/data/ENIGMA/ENIGMA_structural_organised.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alessiogiacomel/Library/CloudStorage/Dropbox/PhD/Analysis/transcriptomics_gio/MetaXcan_TWAS_Analysis/data/ENIGMA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2B76534-46FD-C141-8B6D-C72953AE7A1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92F16F4A-5C98-E94D-81D7-B65501F04B70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="560" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{BF3110D8-B70B-EB46-8D71-9669AD8BE9C5}"/>
+    <workbookView xWindow="760" yWindow="560" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{BF3110D8-B70B-EB46-8D71-9669AD8BE9C5}"/>
   </bookViews>
   <sheets>
     <sheet name="Surface" sheetId="1" r:id="rId1"/>
@@ -58,9 +58,6 @@
     <t>SCZ</t>
   </si>
   <si>
-    <t>Thalamus</t>
-  </si>
-  <si>
     <t>Caudate</t>
   </si>
   <si>
@@ -73,12 +70,6 @@
     <t>Amygdala</t>
   </si>
   <si>
-    <t>Accumbens</t>
-  </si>
-  <si>
-    <t>Pallidus</t>
-  </si>
-  <si>
     <t>OCD</t>
   </si>
   <si>
@@ -290,6 +281,15 @@
   </si>
   <si>
     <t>AN</t>
+  </si>
+  <si>
+    <t>Thalamusproper</t>
+  </si>
+  <si>
+    <t>Accumbensarea</t>
+  </si>
+  <si>
+    <t>Pallidum</t>
   </si>
 </sst>
 </file>
@@ -702,15 +702,15 @@
         <v>5</v>
       </c>
       <c r="F1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B2">
         <v>-7.0000000000000007E-2</v>
@@ -733,7 +733,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B3">
         <v>-0.09</v>
@@ -756,7 +756,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B4">
         <v>-0.13</v>
@@ -779,7 +779,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B5">
         <v>-0.06</v>
@@ -802,7 +802,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B6">
         <v>-7.0000000000000007E-2</v>
@@ -825,7 +825,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B7">
         <v>-0.12</v>
@@ -848,7 +848,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B8">
         <v>-0.11</v>
@@ -871,7 +871,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B9">
         <v>-0.1</v>
@@ -894,7 +894,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B10">
         <v>-0.09</v>
@@ -917,7 +917,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B11">
         <v>-0.11</v>
@@ -940,7 +940,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B12">
         <v>-0.12</v>
@@ -963,7 +963,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B13">
         <v>-7.0000000000000007E-2</v>
@@ -986,7 +986,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B14">
         <v>-0.11</v>
@@ -1009,7 +1009,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B15">
         <v>-0.1</v>
@@ -1032,7 +1032,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B16">
         <v>-0.08</v>
@@ -1055,7 +1055,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B17">
         <v>-0.04</v>
@@ -1078,7 +1078,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B18">
         <v>-0.08</v>
@@ -1101,7 +1101,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B19">
         <v>-0.08</v>
@@ -1124,7 +1124,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B20">
         <v>-0.12</v>
@@ -1147,7 +1147,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B21">
         <v>-0.08</v>
@@ -1170,7 +1170,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B22">
         <v>-0.1</v>
@@ -1193,7 +1193,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B23">
         <v>-0.13</v>
@@ -1216,7 +1216,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B24">
         <v>-0.08</v>
@@ -1239,7 +1239,7 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B25">
         <v>-0.1</v>
@@ -1262,7 +1262,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B26">
         <v>-0.11</v>
@@ -1285,7 +1285,7 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B27">
         <v>-0.12</v>
@@ -1308,7 +1308,7 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B28">
         <v>-0.15</v>
@@ -1331,7 +1331,7 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B29">
         <v>-0.13</v>
@@ -1354,7 +1354,7 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B30">
         <v>-0.11</v>
@@ -1377,7 +1377,7 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B31">
         <v>-0.09</v>
@@ -1400,7 +1400,7 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B32">
         <v>-0.05</v>
@@ -1423,7 +1423,7 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B33">
         <v>-0.11</v>
@@ -1446,7 +1446,7 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B34">
         <v>-0.06</v>
@@ -1469,7 +1469,7 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B35">
         <v>-0.12</v>
@@ -1499,7 +1499,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B94C8F5-6F7E-2C4A-A7C7-23219239FFD9}">
   <dimension ref="A1:H69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
@@ -1525,18 +1525,18 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G1" t="s">
         <v>5</v>
       </c>
       <c r="H1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B2">
         <v>0.01</v>
@@ -1562,7 +1562,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B3">
         <v>-0.11</v>
@@ -1588,7 +1588,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B4">
         <v>-0.02</v>
@@ -1614,7 +1614,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B5">
         <v>0.11</v>
@@ -1640,7 +1640,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B6">
         <v>-0.06</v>
@@ -1666,7 +1666,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B7">
         <v>-0.01</v>
@@ -1692,7 +1692,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B8">
         <v>0.08</v>
@@ -1718,7 +1718,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -1744,7 +1744,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B10">
         <v>0.04</v>
@@ -1770,7 +1770,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B11">
         <v>0.14000000000000001</v>
@@ -1796,7 +1796,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B12">
         <v>0.03</v>
@@ -1822,7 +1822,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B13">
         <v>0.11</v>
@@ -1848,7 +1848,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B14">
         <v>-0.08</v>
@@ -1874,7 +1874,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B15">
         <v>0.02</v>
@@ -1900,7 +1900,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B16">
         <v>0.1</v>
@@ -1926,7 +1926,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B17">
         <v>-0.01</v>
@@ -1952,7 +1952,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B18">
         <v>-0.01</v>
@@ -1978,7 +1978,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B19">
         <v>-0.01</v>
@@ -2004,7 +2004,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B20">
         <v>-0.03</v>
@@ -2030,7 +2030,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B21">
         <v>0.04</v>
@@ -2056,7 +2056,7 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B22">
         <v>0.05</v>
@@ -2082,7 +2082,7 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B23">
         <v>-0.11</v>
@@ -2108,7 +2108,7 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B24">
         <v>-0.06</v>
@@ -2134,7 +2134,7 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B25">
         <v>0.04</v>
@@ -2160,7 +2160,7 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B26">
         <v>-0.09</v>
@@ -2186,7 +2186,7 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B27">
         <v>0.03</v>
@@ -2212,7 +2212,7 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B28">
         <v>-0.04</v>
@@ -2238,7 +2238,7 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B29">
         <v>0.1</v>
@@ -2264,7 +2264,7 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B30">
         <v>0.04</v>
@@ -2290,7 +2290,7 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B31">
         <v>0.02</v>
@@ -2316,7 +2316,7 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B32">
         <v>0.08</v>
@@ -2342,7 +2342,7 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B33">
         <v>-0.02</v>
@@ -2368,7 +2368,7 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B34">
         <v>-0.02</v>
@@ -2394,7 +2394,7 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B35">
         <v>-0.01</v>
@@ -2529,11 +2529,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8098B45E-117C-1144-941A-CC1D17288157}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -2552,18 +2555,18 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G1" t="s">
         <v>5</v>
       </c>
       <c r="H1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>11</v>
+        <v>82</v>
       </c>
       <c r="B2">
         <v>-0.1</v>
@@ -2589,7 +2592,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3">
         <v>-0.14000000000000001</v>
@@ -2615,7 +2618,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4">
         <v>-7.0000000000000007E-2</v>
@@ -2641,7 +2644,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5">
         <v>0.06</v>
@@ -2667,7 +2670,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>12</v>
+        <v>83</v>
       </c>
       <c r="B6">
         <v>0.04</v>
@@ -2693,7 +2696,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7">
         <v>-0.08</v>
@@ -2719,7 +2722,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>6</v>
+        <v>81</v>
       </c>
       <c r="B8">
         <v>-7.0000000000000007E-2</v>

</xml_diff>